<commit_message>
Small modification to slides from chapter #4.  Will eventually move ROC to chapter 5 slides as was done in class. Uploading latest copy of midterm study guide which covers up to slide #8 in chapter #5. Uploading spreadsheet used to calculate teh answers for homework #3. Uploading one image used in the midterm study guide.
</commit_message>
<xml_diff>
--- a/Gradiance Submissions/Homework #3/Homework #3 - Problem Calculations.xlsx
+++ b/Gradiance Submissions/Homework #3/Homework #3 - Problem Calculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="129">
   <si>
     <t>Example</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>P(S,C,H,W|N)</t>
+  </si>
+  <si>
+    <t>P(N|S,C,H,W)</t>
   </si>
 </sst>
 </file>
@@ -812,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N170"/>
+  <dimension ref="A1:M175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K160" sqref="K160"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J160" sqref="J160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -857,6 +860,9 @@
       <c r="E2">
         <v>3</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
       <c r="G2">
         <f>1/(C$2)^2</f>
         <v>1.5624999999999998</v>
@@ -2085,12 +2091,12 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:4">
       <c r="B97" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -2101,7 +2107,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>72</v>
       </c>
@@ -2112,7 +2118,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>73</v>
       </c>
@@ -2124,7 +2130,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>72</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>0.56087803790825519</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>73</v>
       </c>
@@ -2145,7 +2151,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>72</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>0.58677554460716563</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>73</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>72</v>
       </c>
@@ -2175,256 +2181,198 @@
         <v>0.53241334253725348</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
-      <c r="E112" t="s">
-        <v>74</v>
-      </c>
-      <c r="F112" t="s">
-        <v>75</v>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>73</v>
+      </c>
+      <c r="B110">
+        <f>1/SQRT(2*PI()*(C$98)^2)*EXP(-1*(3.12-B$98)^2/(2*(C$98)^2))</f>
+        <v>0.59619472164846865</v>
+      </c>
+      <c r="D110">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>72</v>
+      </c>
+      <c r="B111">
+        <f>1/SQRT(2*PI()*(C$99)^2)*EXP(-1*(3.12-B$99)^2/(2*(C$99)^2))</f>
+        <v>0.57675648862820461</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="B113">
-        <v>52</v>
-      </c>
-      <c r="C113">
-        <v>50</v>
-      </c>
-      <c r="E113">
-        <f>(B113+1)/(SUM(B113:C113)+2)</f>
-        <v>0.50961538461538458</v>
-      </c>
-      <c r="F113">
-        <f>(B113+100/250*2)/(SUM(B113:C113)+2)</f>
-        <v>0.50769230769230766</v>
+        <f>1/SQRT(2*PI()*(C$98)^2)*EXP(-1*(3.14-B$98)^2/(2*(C$98)^2))</f>
+        <v>0.6472868499440434</v>
+      </c>
+      <c r="D113">
+        <v>3.14</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
+        <v>72</v>
+      </c>
+      <c r="B114">
+        <f>1/SQRT(2*PI()*(C$99)^2)*EXP(-1*(3.14-B$99)^2/(2*(C$99)^2))</f>
+        <v>0.56627895717459653</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="E117" t="s">
+        <v>74</v>
+      </c>
+      <c r="F117" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118">
+        <v>52</v>
+      </c>
+      <c r="C118">
+        <v>50</v>
+      </c>
+      <c r="E118">
+        <f>(B118+1)/(SUM(B118:C118)+2)</f>
+        <v>0.50961538461538458</v>
+      </c>
+      <c r="F118">
+        <f>(B118+100/250*2)/(SUM(B118:C118)+2)</f>
+        <v>0.50769230769230766</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" t="s">
         <v>3</v>
       </c>
-      <c r="B114">
+      <c r="B119">
         <v>44</v>
       </c>
-      <c r="C114">
+      <c r="C119">
         <v>16</v>
       </c>
-      <c r="E114">
-        <f t="shared" ref="E114:E116" si="2">(B114+1)/(SUM(B114:C114)+2)</f>
+      <c r="E119">
+        <f t="shared" ref="E119:E121" si="2">(B119+1)/(SUM(B119:C119)+2)</f>
         <v>0.72580645161290325</v>
       </c>
-      <c r="F114">
-        <f t="shared" ref="F114:F116" si="3">(B114+100/250*2)/(SUM(B114:C114)+2)</f>
+      <c r="F119">
+        <f t="shared" ref="F119:F121" si="3">(B119+100/250*2)/(SUM(B119:C119)+2)</f>
         <v>0.72258064516129028</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
-      <c r="A115" t="s">
+    <row r="120" spans="1:6">
+      <c r="A120" t="s">
         <v>5</v>
       </c>
-      <c r="B115">
+      <c r="B120">
         <v>10</v>
       </c>
-      <c r="C115">
+      <c r="C120">
         <v>2</v>
       </c>
-      <c r="E115">
+      <c r="E120">
         <f t="shared" si="2"/>
         <v>0.7857142857142857</v>
       </c>
-      <c r="F115">
+      <c r="F120">
         <f t="shared" si="3"/>
         <v>0.77142857142857146</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
-      <c r="A116" t="s">
+    <row r="121" spans="1:6">
+      <c r="A121" t="s">
         <v>7</v>
       </c>
-      <c r="B116">
+      <c r="B121">
         <v>6</v>
       </c>
-      <c r="C116">
+      <c r="C121">
         <v>4</v>
       </c>
-      <c r="E116">
+      <c r="E121">
         <f t="shared" si="2"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="F116">
+      <c r="F121">
         <f t="shared" si="3"/>
         <v>0.56666666666666665</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
-      <c r="B122" t="s">
+    <row r="127" spans="1:6">
+      <c r="B127" t="s">
         <v>76</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C127" t="s">
         <v>78</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D127" t="s">
         <v>79</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E127" t="s">
         <v>80</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F127" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123">
-        <v>1</v>
-      </c>
-      <c r="B123" t="s">
-        <v>70</v>
-      </c>
-      <c r="C123" t="s">
-        <v>13</v>
-      </c>
-      <c r="D123" t="s">
-        <v>13</v>
-      </c>
-      <c r="E123" t="s">
-        <v>83</v>
-      </c>
-      <c r="F123" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124">
-        <v>2</v>
-      </c>
-      <c r="B124" t="s">
-        <v>70</v>
-      </c>
-      <c r="C124" t="s">
-        <v>13</v>
-      </c>
-      <c r="D124" t="s">
-        <v>13</v>
-      </c>
-      <c r="E124" t="s">
-        <v>70</v>
-      </c>
-      <c r="F124" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125">
-        <v>3</v>
-      </c>
-      <c r="B125" t="s">
-        <v>77</v>
-      </c>
-      <c r="C125" t="s">
-        <v>13</v>
-      </c>
-      <c r="D125" t="s">
-        <v>13</v>
-      </c>
-      <c r="E125" t="s">
-        <v>83</v>
-      </c>
-      <c r="F125" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126">
-        <v>4</v>
-      </c>
-      <c r="B126" t="s">
-        <v>56</v>
-      </c>
-      <c r="C126" t="s">
-        <v>18</v>
-      </c>
-      <c r="D126" t="s">
-        <v>13</v>
-      </c>
-      <c r="E126" t="s">
-        <v>83</v>
-      </c>
-      <c r="F126" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127">
-        <v>5</v>
-      </c>
-      <c r="B127" t="s">
-        <v>56</v>
-      </c>
-      <c r="C127" t="s">
-        <v>7</v>
-      </c>
-      <c r="D127" t="s">
-        <v>19</v>
-      </c>
-      <c r="E127" t="s">
-        <v>83</v>
-      </c>
-      <c r="F127" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B128" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C128" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D128" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E128" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F128" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:14">
+    <row r="129" spans="1:6">
       <c r="A129">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B129" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C129" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D129" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E129" t="s">
         <v>70</v>
       </c>
       <c r="F129" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="130" spans="1:14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B130" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C130" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D130" t="s">
         <v>13</v>
@@ -2433,21 +2381,21 @@
         <v>83</v>
       </c>
       <c r="F130" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="131" spans="1:14">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B131" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C131" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D131" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E131" t="s">
         <v>83</v>
@@ -2456,15 +2404,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="132" spans="1:14">
+    <row r="132" spans="1:6">
       <c r="A132">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B132" t="s">
         <v>56</v>
       </c>
       <c r="C132" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D132" t="s">
         <v>19</v>
@@ -2476,15 +2424,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="133" spans="1:14">
+    <row r="133" spans="1:6">
       <c r="A133">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C133" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D133" t="s">
         <v>19</v>
@@ -2493,21 +2441,21 @@
         <v>70</v>
       </c>
       <c r="F133" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="134" spans="1:14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B134" t="s">
         <v>77</v>
       </c>
       <c r="C134" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D134" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E134" t="s">
         <v>70</v>
@@ -2516,295 +2464,213 @@
         <v>82</v>
       </c>
     </row>
-    <row r="135" spans="1:14">
+    <row r="135" spans="1:6">
       <c r="A135">
+        <v>8</v>
+      </c>
+      <c r="B135" t="s">
+        <v>70</v>
+      </c>
+      <c r="C135" t="s">
+        <v>18</v>
+      </c>
+      <c r="D135" t="s">
         <v>13</v>
-      </c>
-      <c r="B135" t="s">
-        <v>77</v>
-      </c>
-      <c r="C135" t="s">
-        <v>13</v>
-      </c>
-      <c r="D135" t="s">
-        <v>19</v>
       </c>
       <c r="E135" t="s">
         <v>83</v>
       </c>
       <c r="F135" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136">
+        <v>9</v>
+      </c>
+      <c r="B136" t="s">
+        <v>70</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" t="s">
+        <v>19</v>
+      </c>
+      <c r="E136" t="s">
+        <v>83</v>
+      </c>
+      <c r="F136" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="136" spans="1:14">
-      <c r="A136">
+    <row r="137" spans="1:6">
+      <c r="A137">
+        <v>10</v>
+      </c>
+      <c r="B137" t="s">
+        <v>56</v>
+      </c>
+      <c r="C137" t="s">
+        <v>18</v>
+      </c>
+      <c r="D137" t="s">
+        <v>19</v>
+      </c>
+      <c r="E137" t="s">
+        <v>83</v>
+      </c>
+      <c r="F137" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138">
+        <v>11</v>
+      </c>
+      <c r="B138" t="s">
+        <v>70</v>
+      </c>
+      <c r="C138" t="s">
+        <v>18</v>
+      </c>
+      <c r="D138" t="s">
+        <v>19</v>
+      </c>
+      <c r="E138" t="s">
+        <v>70</v>
+      </c>
+      <c r="F138" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139">
+        <v>12</v>
+      </c>
+      <c r="B139" t="s">
+        <v>77</v>
+      </c>
+      <c r="C139" t="s">
+        <v>18</v>
+      </c>
+      <c r="D139" t="s">
+        <v>13</v>
+      </c>
+      <c r="E139" t="s">
+        <v>70</v>
+      </c>
+      <c r="F139" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140">
+        <v>13</v>
+      </c>
+      <c r="B140" t="s">
+        <v>77</v>
+      </c>
+      <c r="C140" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" t="s">
+        <v>19</v>
+      </c>
+      <c r="E140" t="s">
+        <v>83</v>
+      </c>
+      <c r="F140" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141">
         <v>14</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B141" t="s">
         <v>56</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C141" t="s">
         <v>18</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D141" t="s">
         <v>13</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E141" t="s">
         <v>70</v>
       </c>
-      <c r="F136" t="s">
+      <c r="F141" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="1:14">
-      <c r="A139" t="s">
+    <row r="144" spans="1:6">
+      <c r="A144" t="s">
         <v>110</v>
       </c>
-      <c r="B139">
-        <f>COUNTIF(F$123:F$136,"Y")/14</f>
+      <c r="B144">
+        <f>COUNTIF(F$128:F$141,"Y")/14</f>
         <v>0.6428571428571429</v>
       </c>
-      <c r="C139">
-        <f>B139*14</f>
+      <c r="C144">
+        <f>B144*14</f>
         <v>9</v>
       </c>
-      <c r="L139" t="s">
-        <v>111</v>
-      </c>
-      <c r="M139">
-        <f>$B$142*$B$148*$B$150*$B$153</f>
-        <v>2.9154518950437316E-2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14">
-      <c r="A140" t="s">
+    </row>
+    <row r="145" spans="1:13">
+      <c r="A145" t="s">
         <v>88</v>
       </c>
-      <c r="B140">
-        <f>COUNTIF(F$123:F$136,"N")/14</f>
+      <c r="B145">
+        <f>COUNTIF(F$128:F$141,"N")/14</f>
         <v>0.35714285714285715</v>
       </c>
-      <c r="C140">
-        <f>B140*14</f>
+      <c r="C145">
+        <f>B145*14</f>
         <v>5</v>
-      </c>
-      <c r="L140" t="s">
-        <v>112</v>
-      </c>
-      <c r="M140">
-        <f>$E$142*$E$148*$E$150*$E$153</f>
-        <v>9.6428571428571447E-2</v>
-      </c>
-      <c r="N140" t="e">
-        <f>SUMPRODUCT(($B$123:$B$136="S")*($C$123:$C$136="C")*($D$123:$D$136="H")*($E$123:$E$136="W")*($F$123:$F$136="Y"))/SUMPRODUCT(($B$123:$B$136="S")*($C$123:$C$136="C")*($D$123:$D$136="H")*($E$123:$E$136="W"))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14">
-      <c r="L141" t="s">
-        <v>110</v>
-      </c>
-      <c r="M141">
-        <f>$B$139</f>
-        <v>0.6428571428571429</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14">
-      <c r="A142" t="s">
-        <v>23</v>
-      </c>
-      <c r="B142">
-        <f>COUNTIF(B$123:B$136,"S")/14</f>
-        <v>0.35714285714285715</v>
-      </c>
-      <c r="C142">
-        <f t="shared" ref="C142:C154" si="4">B142*14</f>
-        <v>5</v>
-      </c>
-      <c r="D142" t="s">
-        <v>91</v>
-      </c>
-      <c r="E142">
-        <f>SUMPRODUCT(($B$123:$B$136="S")*($F$123:$F$136="Y"))/COUNTIF($B$123:$B$136,"S")</f>
-        <v>0.4</v>
-      </c>
-      <c r="F142">
-        <f>E142*COUNTIF($B$123:$B$136,"S")</f>
-        <v>2</v>
-      </c>
-      <c r="G142" t="s">
-        <v>94</v>
-      </c>
-      <c r="H142">
-        <f>SUMPRODUCT(($B$123:$B$136="S")*($F$123:$F$136="N"))/COUNTIF($B$123:$B$136,"S")</f>
-        <v>0.6</v>
-      </c>
-      <c r="I142">
-        <f>H142*COUNTIF($B$123:$B$136,"S")</f>
-        <v>3</v>
-      </c>
-      <c r="M142">
-        <f>M140*M139/M141</f>
-        <v>4.3731778425655978E-3</v>
-      </c>
-      <c r="N142">
-        <f>4/243</f>
-        <v>1.646090534979424E-2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14">
-      <c r="A143" t="s">
-        <v>84</v>
-      </c>
-      <c r="B143">
-        <f>COUNTIF(B$123:B$136,"O")/14</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="C143">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="D143" t="s">
-        <v>92</v>
-      </c>
-      <c r="E143">
-        <f>SUMPRODUCT(($B$123:$B$136="O")*($F$123:$F$136="Y"))/COUNTIF($B$123:$B$136,"O")</f>
-        <v>1</v>
-      </c>
-      <c r="F143">
-        <f>E143*COUNTIF($B$123:$B$136,"O")</f>
-        <v>4</v>
-      </c>
-      <c r="G143" t="s">
-        <v>95</v>
-      </c>
-      <c r="H143">
-        <f>SUMPRODUCT(($B$123:$B$136="O")*($F$123:$F$136="N"))/COUNTIF($B$123:$B$136,"O")</f>
-        <v>0</v>
-      </c>
-      <c r="I143">
-        <f>H143*COUNTIF($B$123:$B$136,"O")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14">
-      <c r="A144" t="s">
-        <v>85</v>
-      </c>
-      <c r="B144">
-        <f>COUNTIF(B$123:B$136,"R")/14</f>
-        <v>0.35714285714285715</v>
-      </c>
-      <c r="C144">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="D144" t="s">
-        <v>93</v>
-      </c>
-      <c r="E144">
-        <f>SUMPRODUCT(($B$123:$B$136="R")*($F$123:$F$136="Y"))/COUNTIF($B$123:$B$136,"R")</f>
-        <v>0.6</v>
-      </c>
-      <c r="F144">
-        <f>E144*COUNTIF($B$123:$B$136,"R")</f>
-        <v>3</v>
-      </c>
-      <c r="G144" t="s">
-        <v>96</v>
-      </c>
-      <c r="H144">
-        <f>SUMPRODUCT(($B$123:$B$136="R")*($F$123:$F$136="N"))/COUNTIF($B$123:$B$136,"R")</f>
-        <v>0.4</v>
-      </c>
-      <c r="I144">
-        <f>H144*COUNTIF($B$123:$B$136,"R")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="146" spans="1:13">
-      <c r="A146" t="s">
-        <v>86</v>
-      </c>
-      <c r="B146">
-        <f>COUNTIF(C$123:C$136,"H")/14</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="C146">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="D146" t="s">
-        <v>97</v>
-      </c>
-      <c r="E146">
-        <f>SUMPRODUCT(($C$123:$C$136="H")*($F$123:$F$136="Y"))/COUNTIF($C$123:$C$136,"H")</f>
-        <v>0.5</v>
-      </c>
-      <c r="F146">
-        <f>E146*COUNTIF($C$123:$C$136,"H")</f>
-        <v>2</v>
-      </c>
-      <c r="G146" t="s">
-        <v>100</v>
-      </c>
-      <c r="H146">
-        <f>SUMPRODUCT(($C$123:$C$136="H")*($F$123:$F$136="N"))/COUNTIF($C$123:$C$136,"H")</f>
-        <v>0.5</v>
-      </c>
-      <c r="I146">
-        <f>H146*COUNTIF($C$123:$C$136,"H")</f>
-        <v>2</v>
-      </c>
-      <c r="L146" t="s">
-        <v>107</v>
-      </c>
-      <c r="M146">
-        <f>$H$142*$H$148*$H$150*$H$153</f>
-        <v>2.1428571428571425E-2</v>
       </c>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B147">
-        <f>COUNTIF(C$123:C$136,"M")/14</f>
-        <v>0.42857142857142855</v>
+        <f>COUNTIF(B$128:B$141,"S")/14</f>
+        <v>0.35714285714285715</v>
       </c>
       <c r="C147">
-        <f t="shared" si="4"/>
-        <v>6</v>
+        <f t="shared" ref="C147:C159" si="4">B147*14</f>
+        <v>5</v>
       </c>
       <c r="D147" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E147">
-        <f>SUMPRODUCT(($C$123:$C$136="M")*($F$123:$F$136="Y"))/COUNTIF($C$123:$C$136,"M")</f>
-        <v>0.66666666666666663</v>
+        <f>SUMPRODUCT(($B$128:$B$141="S")*($F$128:$F$141="Y"))/COUNTIF($B$128:$B$141,"S")</f>
+        <v>0.4</v>
       </c>
       <c r="F147">
-        <f>E147*COUNTIF($C$123:$C$136,"M")</f>
-        <v>4</v>
+        <f>E147*COUNTIF($B$128:$B$141,"S")</f>
+        <v>2</v>
       </c>
       <c r="G147" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="H147">
-        <f>SUMPRODUCT(($C$123:$C$136="M")*($F$123:$F$136="N"))/COUNTIF($C$123:$C$136,"M")</f>
-        <v>0.33333333333333331</v>
+        <f>SUMPRODUCT(($B$128:$B$141="S")*($F$128:$F$141="N"))/COUNTIF($B$128:$B$141,"S")</f>
+        <v>0.6</v>
       </c>
       <c r="I147">
-        <f>H147*COUNTIF($C$123:$C$136,"M")</f>
-        <v>2</v>
+        <f>H147*COUNTIF($B$128:$B$141,"S")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B148">
-        <f>COUNTIF(C$123:C$136,"C")/14</f>
+        <f>COUNTIF(B$128:B$141,"O")/14</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="C148">
@@ -2812,339 +2678,530 @@
         <v>4</v>
       </c>
       <c r="D148" t="s">
+        <v>92</v>
+      </c>
+      <c r="E148">
+        <f>SUMPRODUCT(($B$128:$B$141="O")*($F$128:$F$141="Y"))/COUNTIF($B$128:$B$141,"O")</f>
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <f>E148*COUNTIF($B$128:$B$141,"O")</f>
+        <v>4</v>
+      </c>
+      <c r="G148" t="s">
+        <v>95</v>
+      </c>
+      <c r="H148">
+        <f>SUMPRODUCT(($B$128:$B$141="O")*($F$128:$F$141="N"))/COUNTIF($B$128:$B$141,"O")</f>
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <f>H148*COUNTIF($B$128:$B$141,"O")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13">
+      <c r="A149" t="s">
+        <v>85</v>
+      </c>
+      <c r="B149">
+        <f>COUNTIF(B$128:B$141,"R")/14</f>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="D149" t="s">
+        <v>93</v>
+      </c>
+      <c r="E149">
+        <f>SUMPRODUCT(($B$128:$B$141="R")*($F$128:$F$141="Y"))/COUNTIF($B$128:$B$141,"R")</f>
+        <v>0.6</v>
+      </c>
+      <c r="F149">
+        <f>E149*COUNTIF($B$128:$B$141,"R")</f>
+        <v>3</v>
+      </c>
+      <c r="G149" t="s">
+        <v>96</v>
+      </c>
+      <c r="H149">
+        <f>SUMPRODUCT(($B$128:$B$141="R")*($F$128:$F$141="N"))/COUNTIF($B$128:$B$141,"R")</f>
+        <v>0.4</v>
+      </c>
+      <c r="I149">
+        <f>H149*COUNTIF($B$128:$B$141,"R")</f>
+        <v>2</v>
+      </c>
+      <c r="L149">
+        <f>B144*L163</f>
+        <v>1.0582010582010581E-2</v>
+      </c>
+      <c r="M149">
+        <f>SUM(L149:L150)/L151</f>
+        <v>0.83336296296296297</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13">
+      <c r="L150">
+        <f>L164*B145</f>
+        <v>1.3714285714285715E-2</v>
+      </c>
+      <c r="M150">
+        <f>SUM(L149:L150)</f>
+        <v>2.4296296296296295E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13">
+      <c r="A151" t="s">
+        <v>86</v>
+      </c>
+      <c r="B151">
+        <f>COUNTIF(C$128:C$141,"H")/14</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D151" t="s">
+        <v>97</v>
+      </c>
+      <c r="E151">
+        <f>SUMPRODUCT(($C$128:$C$141="H")*($F$128:$F$141="Y"))/COUNTIF($C$128:$C$141,"H")</f>
+        <v>0.5</v>
+      </c>
+      <c r="F151">
+        <f>E151*COUNTIF($C$128:$C$141,"H")</f>
+        <v>2</v>
+      </c>
+      <c r="G151" t="s">
+        <v>100</v>
+      </c>
+      <c r="H151">
+        <f>SUMPRODUCT(($C$128:$C$141="H")*($F$128:$F$141="N"))/COUNTIF($C$128:$C$141,"H")</f>
+        <v>0.5</v>
+      </c>
+      <c r="I151">
+        <f>H151*COUNTIF($C$128:$C$141,"H")</f>
+        <v>2</v>
+      </c>
+      <c r="K151" t="s">
+        <v>111</v>
+      </c>
+      <c r="L151">
+        <f>B147*B153*B155*B158</f>
+        <v>2.9154518950437316E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13">
+      <c r="A152" t="s">
+        <v>21</v>
+      </c>
+      <c r="B152">
+        <f>COUNTIF(C$128:C$141,"M")/14</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="C152">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="D152" t="s">
+        <v>98</v>
+      </c>
+      <c r="E152">
+        <f>SUMPRODUCT(($C$128:$C$141="M")*($F$128:$F$141="Y"))/COUNTIF($C$128:$C$141,"M")</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F152">
+        <f>E152*COUNTIF($C$128:$C$141,"M")</f>
+        <v>4</v>
+      </c>
+      <c r="G152" t="s">
+        <v>101</v>
+      </c>
+      <c r="H152">
+        <f>SUMPRODUCT(($C$128:$C$141="M")*($F$128:$F$141="N"))/COUNTIF($C$128:$C$141,"M")</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I152">
+        <f>H152*COUNTIF($C$128:$C$141,"M")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13">
+      <c r="A153" t="s">
+        <v>87</v>
+      </c>
+      <c r="B153">
+        <f>COUNTIF(C$128:C$141,"C")/14</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="C153">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D153" t="s">
         <v>99</v>
       </c>
-      <c r="E148">
-        <f>SUMPRODUCT(($C$123:$C$136="C")*($F$123:$F$136="Y"))/COUNTIF($C$123:$C$136,"C")</f>
+      <c r="E153">
+        <f>SUMPRODUCT(($C$128:$C$141="C")*($F$128:$F$141="Y"))/COUNTIF($C$128:$C$141,"C")</f>
         <v>0.75</v>
       </c>
-      <c r="F148">
-        <f>E148*COUNTIF($C$123:$C$136,"C")</f>
+      <c r="F153">
+        <f>E153*COUNTIF($C$128:$C$141,"C")</f>
         <v>3</v>
       </c>
-      <c r="G148" t="s">
+      <c r="G153" t="s">
         <v>102</v>
       </c>
-      <c r="H148">
-        <f>SUMPRODUCT(($C$123:$C$136="C")*($F$123:$F$136="N"))/COUNTIF($C$123:$C$136,"C")</f>
+      <c r="H153">
+        <f>SUMPRODUCT(($C$128:$C$141="C")*($F$128:$F$141="N"))/COUNTIF($C$128:$C$141,"C")</f>
         <v>0.25</v>
       </c>
-      <c r="I148">
-        <f>H148*COUNTIF($C$123:$C$136,"C")</f>
+      <c r="I153">
+        <f>H153*COUNTIF($C$128:$C$141,"C")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
-      <c r="A150" t="s">
+    <row r="155" spans="1:13">
+      <c r="A155" t="s">
         <v>86</v>
       </c>
-      <c r="B150">
-        <f>COUNTIF(D$123:D$136,"H")/14</f>
+      <c r="B155">
+        <f>COUNTIF(D$128:D$141,"H")/14</f>
         <v>0.5</v>
       </c>
-      <c r="C150">
+      <c r="C155">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D155" t="s">
         <v>97</v>
       </c>
-      <c r="E150">
-        <f>SUMPRODUCT(($D$123:$D$136="H")*($F$123:$F$136="Y"))/COUNTIF($D$123:$D$136,"H")</f>
+      <c r="E155">
+        <f>SUMPRODUCT(($D$128:$D$141="H")*($F$128:$F$141="Y"))/COUNTIF($D$128:$D$141,"H")</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="F150">
-        <f>E150*COUNTIF($D$123:$D$136,"H")</f>
+      <c r="F155">
+        <f>E155*COUNTIF($D$128:$D$141,"H")</f>
         <v>3</v>
       </c>
-      <c r="G150" t="s">
+      <c r="G155" t="s">
         <v>100</v>
       </c>
-      <c r="H150">
-        <f>SUMPRODUCT(($D$123:$D$136="H")*($F$123:$F$136="N"))/COUNTIF($D$123:$D$136,"H")</f>
+      <c r="H155">
+        <f>SUMPRODUCT(($D$128:$D$141="H")*($F$128:$F$141="N"))/COUNTIF($D$128:$D$141,"H")</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="I150">
-        <f>H150*COUNTIF($D$123:$D$136,"H")</f>
+      <c r="I155">
+        <f>H155*COUNTIF($D$128:$D$141,"H")</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="151" spans="1:13">
-      <c r="A151" t="s">
+      <c r="K155" t="s">
+        <v>112</v>
+      </c>
+      <c r="L155">
+        <f>L163*B144/M150</f>
+        <v>0.43554006968641112</v>
+      </c>
+      <c r="M155">
+        <f>SUM(L155:L156)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13">
+      <c r="A156" t="s">
         <v>88</v>
       </c>
-      <c r="B151">
-        <f>COUNTIF(D$123:D$136,"N")/14</f>
+      <c r="B156">
+        <f>COUNTIF(D$128:D$141,"N")/14</f>
         <v>0.5</v>
       </c>
-      <c r="C151">
+      <c r="C156">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D156" t="s">
         <v>103</v>
       </c>
-      <c r="E151">
-        <f>SUMPRODUCT(($D$123:$D$136="N")*($F$123:$F$136="Y"))/COUNTIF($D$123:$D$136,"N")</f>
+      <c r="E156">
+        <f>SUMPRODUCT(($D$128:$D$141="N")*($F$128:$F$141="Y"))/COUNTIF($D$128:$D$141,"N")</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="F151">
-        <f>E151*COUNTIF($D$123:$D$136,"N")</f>
+      <c r="F156">
+        <f>E156*COUNTIF($D$128:$D$141,"N")</f>
         <v>6</v>
       </c>
-      <c r="G151" t="s">
+      <c r="G156" t="s">
         <v>104</v>
       </c>
-      <c r="H151">
-        <f>SUMPRODUCT(($D$123:$D$136="N")*($F$123:$F$136="N"))/COUNTIF($D$123:$D$136,"N")</f>
+      <c r="H156">
+        <f>SUMPRODUCT(($D$128:$D$141="N")*($F$128:$F$141="N"))/COUNTIF($D$128:$D$141,"N")</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="I151">
-        <f>H151*COUNTIF($D$123:$D$136,"N")</f>
+      <c r="I156">
+        <f>H156*COUNTIF($D$128:$D$141,"N")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:13">
-      <c r="A153" t="s">
+      <c r="K156" t="s">
+        <v>128</v>
+      </c>
+      <c r="L156">
+        <f>L164*B145/M150</f>
+        <v>0.56445993031358888</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13">
+      <c r="A158" t="s">
         <v>89</v>
       </c>
-      <c r="B153">
-        <f>COUNTIF(E$123:E$136,"W")/14</f>
+      <c r="B158">
+        <f>COUNTIF(E$128:E$141,"W")/14</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="C153">
+      <c r="C158">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D158" t="s">
         <v>105</v>
       </c>
-      <c r="E153">
-        <f>SUMPRODUCT(($E$123:$E$136="W")*($F$123:$F$136="Y"))/COUNTIF($E$123:$E$136,"W")</f>
+      <c r="E158">
+        <f>SUMPRODUCT(($E$128:$E$141="W")*($F$128:$F$141="Y"))/COUNTIF($E$128:$E$141,"W")</f>
         <v>0.75</v>
       </c>
-      <c r="F153">
-        <f>E153*COUNTIF($E$123:$E$136,"W")</f>
+      <c r="F158">
+        <f>E158*COUNTIF($E$128:$E$141,"W")</f>
         <v>6</v>
       </c>
-      <c r="G153" t="s">
+      <c r="G158" t="s">
         <v>106</v>
       </c>
-      <c r="H153">
-        <f>SUMPRODUCT(($E$123:$E$136="W")*($F$123:$F$136="N"))/COUNTIF($E$123:$E$136,"W")</f>
+      <c r="H158">
+        <f>SUMPRODUCT(($E$128:$E$141="W")*($F$128:$F$141="N"))/COUNTIF($E$128:$E$141,"W")</f>
         <v>0.25</v>
       </c>
-      <c r="I153">
-        <f>H153*COUNTIF($E$123:$E$136,"W")</f>
+      <c r="I158">
+        <f>H158*COUNTIF($E$128:$E$141,"W")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
-      <c r="A154" t="s">
+    <row r="159" spans="1:13">
+      <c r="A159" t="s">
         <v>23</v>
       </c>
-      <c r="B154">
-        <f>COUNTIF(E$123:E$136,"S")/14</f>
+      <c r="B159">
+        <f>COUNTIF(E$128:E$141,"S")/14</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="C154">
+      <c r="C159">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D159" t="s">
         <v>91</v>
       </c>
-      <c r="E154">
-        <f>SUMPRODUCT(($E$123:$E$136="S")*($F$123:$F$136="Y"))/COUNTIF($E$123:$E$136,"S")</f>
+      <c r="E159">
+        <f>SUMPRODUCT(($E$128:$E$141="S")*($F$128:$F$141="Y"))/COUNTIF($E$128:$E$141,"S")</f>
         <v>0.5</v>
       </c>
-      <c r="F154">
-        <f>E154*COUNTIF($E$123:$E$136,"S")</f>
+      <c r="F159">
+        <f>E159*COUNTIF($E$128:$E$141,"S")</f>
         <v>3</v>
       </c>
-      <c r="G154" t="s">
+      <c r="G159" t="s">
         <v>94</v>
       </c>
-      <c r="H154">
-        <f>SUMPRODUCT(($E$123:$E$136="S")*($F$123:$F$136="N"))/COUNTIF($E$123:$E$136,"S")</f>
+      <c r="H159">
+        <f>SUMPRODUCT(($E$128:$E$141="S")*($F$128:$F$141="N"))/COUNTIF($E$128:$E$141,"S")</f>
         <v>0.5</v>
       </c>
-      <c r="I154">
-        <f>H154*COUNTIF($E$123:$E$136,"S")</f>
+      <c r="I159">
+        <f>H159*COUNTIF($E$128:$E$141,"S")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
-      <c r="D158" t="s">
+    <row r="163" spans="4:13">
+      <c r="D163" t="s">
         <v>90</v>
       </c>
-      <c r="E158">
-        <f>SUMPRODUCT(($B$123:$B$136="S")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E163">
+        <f>SUMPRODUCT(($B$128:$B$141="S")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="G158" t="s">
+      <c r="G163" t="s">
         <v>120</v>
       </c>
-      <c r="H158">
-        <f>SUMPRODUCT(($B$123:$B$136="S")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H163">
+        <f>SUMPRODUCT(($B$128:$B$141="S")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.6</v>
       </c>
-      <c r="K158" t="s">
+      <c r="K163" t="s">
         <v>107</v>
       </c>
-      <c r="L158">
-        <f>$E$158*$E$164*$E$166*$E$169</f>
+      <c r="L163">
+        <f>$E$163*$E$169*$E$171*$E$174</f>
         <v>1.6460905349794237E-2</v>
       </c>
-    </row>
-    <row r="159" spans="1:13">
-      <c r="D159" t="s">
+      <c r="M163">
+        <f>4/243</f>
+        <v>1.646090534979424E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="4:13">
+      <c r="D164" t="s">
         <v>113</v>
       </c>
-      <c r="E159">
-        <f>SUMPRODUCT(($B$123:$B$136="O")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E164">
+        <f>SUMPRODUCT(($B$128:$B$141="O")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="G159" t="s">
+      <c r="G164" t="s">
         <v>121</v>
       </c>
-      <c r="H159">
-        <f>SUMPRODUCT(($B$123:$B$136="O")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H164">
+        <f>SUMPRODUCT(($B$128:$B$141="O")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0</v>
       </c>
-      <c r="K159" t="s">
+      <c r="K164" t="s">
         <v>127</v>
       </c>
-      <c r="L159">
-        <f>$H$158*$H$164*$H$166*$H$169</f>
+      <c r="L164">
+        <f>$H$163*$H$169*$H$171*$H$174</f>
         <v>3.8400000000000004E-2</v>
       </c>
-    </row>
-    <row r="160" spans="1:13">
-      <c r="D160" t="s">
+      <c r="M164">
+        <f>24/625</f>
+        <v>3.8399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="4:13">
+      <c r="D165" t="s">
         <v>114</v>
       </c>
-      <c r="E160">
-        <f>SUMPRODUCT(($B$123:$B$136="R")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E165">
+        <f>SUMPRODUCT(($B$128:$B$141="R")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G160" t="s">
+      <c r="G165" t="s">
         <v>122</v>
       </c>
-      <c r="H160">
-        <f>SUMPRODUCT(($B$123:$B$136="R")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H165">
+        <f>SUMPRODUCT(($B$128:$B$141="R")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="162" spans="4:8">
-      <c r="D162" t="s">
+    <row r="167" spans="4:13">
+      <c r="D167" t="s">
         <v>115</v>
       </c>
-      <c r="E162">
-        <f>SUMPRODUCT(($C$123:$C$136="H")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E167">
+        <f>SUMPRODUCT(($C$128:$C$141="H")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="G162" t="s">
+      <c r="G167" t="s">
         <v>123</v>
       </c>
-      <c r="H162">
-        <f>SUMPRODUCT(($C$123:$C$136="H")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H167">
+        <f>SUMPRODUCT(($C$128:$C$141="H")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="163" spans="4:8">
-      <c r="D163" t="s">
+    <row r="168" spans="4:13">
+      <c r="D168" t="s">
         <v>116</v>
       </c>
-      <c r="E163">
-        <f>SUMPRODUCT(($C$123:$C$136="M")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E168">
+        <f>SUMPRODUCT(($C$128:$C$141="M")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="G163" t="s">
+      <c r="G168" t="s">
         <v>124</v>
       </c>
-      <c r="H163">
-        <f>SUMPRODUCT(($C$123:$C$136="M")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H168">
+        <f>SUMPRODUCT(($C$128:$C$141="M")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="164" spans="4:8">
-      <c r="D164" t="s">
+    <row r="169" spans="4:13">
+      <c r="D169" t="s">
         <v>117</v>
       </c>
-      <c r="E164">
-        <f>SUMPRODUCT(($C$123:$C$136="C")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E169">
+        <f>SUMPRODUCT(($C$128:$C$141="C")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G164" t="s">
+      <c r="G169" t="s">
         <v>125</v>
       </c>
-      <c r="H164">
-        <f>SUMPRODUCT(($C$123:$C$136="C")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H169">
+        <f>SUMPRODUCT(($C$128:$C$141="C")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="166" spans="4:8">
-      <c r="D166" t="s">
+    <row r="171" spans="4:13">
+      <c r="D171" t="s">
         <v>115</v>
       </c>
-      <c r="E166">
-        <f>SUMPRODUCT(($D$123:$D$136="H")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E171">
+        <f>SUMPRODUCT(($D$128:$D$141="H")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G166" t="s">
+      <c r="G171" t="s">
         <v>123</v>
       </c>
-      <c r="H166">
-        <f>SUMPRODUCT(($D$123:$D$136="H")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H171">
+        <f>SUMPRODUCT(($D$128:$D$141="H")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="167" spans="4:8">
-      <c r="D167" t="s">
+    <row r="172" spans="4:13">
+      <c r="D172" t="s">
         <v>118</v>
       </c>
-      <c r="E167">
-        <f>SUMPRODUCT(($D$123:$D$136="N")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E172">
+        <f>SUMPRODUCT(($D$128:$D$141="N")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G167" t="s">
+      <c r="G172" t="s">
         <v>88</v>
       </c>
-      <c r="H167">
-        <f>SUMPRODUCT(($D$123:$D$136="N")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H172">
+        <f>SUMPRODUCT(($D$128:$D$141="N")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="169" spans="4:8">
-      <c r="D169" t="s">
+    <row r="174" spans="4:13">
+      <c r="D174" t="s">
         <v>119</v>
       </c>
-      <c r="E169">
-        <f>SUMPRODUCT(($E$123:$E$136="W")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E174">
+        <f>SUMPRODUCT(($E$128:$E$141="W")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G169" t="s">
+      <c r="G174" t="s">
         <v>126</v>
       </c>
-      <c r="H169">
-        <f>SUMPRODUCT(($E$123:$E$136="W")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H174">
+        <f>SUMPRODUCT(($E$128:$E$141="W")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="170" spans="4:8">
-      <c r="D170" t="s">
+    <row r="175" spans="4:13">
+      <c r="D175" t="s">
         <v>90</v>
       </c>
-      <c r="E170">
-        <f>SUMPRODUCT(($E$123:$E$136="S")*($F$123:$F$136="Y"))/COUNTIF($F$123:$F$136,"Y")</f>
+      <c r="E175">
+        <f>SUMPRODUCT(($E$128:$E$141="S")*($F$128:$F$141="Y"))/COUNTIF($F$128:$F$141,"Y")</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G170" t="s">
+      <c r="G175" t="s">
         <v>120</v>
       </c>
-      <c r="H170">
-        <f>SUMPRODUCT(($E$123:$E$136="S")*($F$123:$F$136="N"))/COUNTIF($F$123:$F$136,"N")</f>
+      <c r="H175">
+        <f>SUMPRODUCT(($E$128:$E$141="S")*($F$128:$F$141="N"))/COUNTIF($F$128:$F$141,"N")</f>
         <v>0.6</v>
       </c>
     </row>

</xml_diff>